<commit_message>
committed by Aziz Ahmed
</commit_message>
<xml_diff>
--- a/PayrollProject/OutPutTestResult/ApprenticeshipLevy Scenarios Test result.xlsx
+++ b/PayrollProject/OutPutTestResult/ApprenticeshipLevy Scenarios Test result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AzizMugdal\git\24-7PeopleXCDPayroll\PayrollProject\OutPutTestResult\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3CE573-F04C-4C72-AE63-451D5FD436D3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55033B97-1E96-4183-B32E-2EC7A712955F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15990" windowWidth="19095" windowHeight="7275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="18510" windowWidth="19095" windowHeight="7275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NormalMonthly" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="102">
   <si>
     <t>AutomationEmployeeNames</t>
   </si>
@@ -575,7 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -719,9 +719,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -735,6 +732,19 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1020,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1125,19 +1135,19 @@
         <v>8</v>
       </c>
       <c r="B4" s="19"/>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="68" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="26" t="s">
+      <c r="E4" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="68" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="27"/>
@@ -1247,21 +1257,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470C2178-89E3-40F8-89C6-280A1D52CB08}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
-    <col min="6" max="7" width="30.7109375" customWidth="1"/>
-    <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" customWidth="1"/>
-    <col min="10" max="10" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" customHeight="1">
@@ -1274,25 +1285,25 @@
       <c r="C1" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="61" t="s">
+      <c r="H1" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="62" t="s">
+      <c r="I1" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="60" t="s">
+      <c r="J1" s="59" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1303,7 +1314,7 @@
       <c r="B2" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="62" t="s">
         <v>93</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -1318,13 +1329,13 @@
       <c r="G2" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="61" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="61" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="61" t="s">
+      <c r="H2" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="60" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1333,26 +1344,58 @@
       <c r="B3" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="64" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="27.75" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
+      <c r="C4" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="44" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1370,11 +1413,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="4" width="32.42578125" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="32.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1">
@@ -1384,16 +1427,16 @@
       <c r="B1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="60" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1402,8 +1445,8 @@
         <v>4</v>
       </c>
       <c r="B2" s="25"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="46" t="s">
         <v>99</v>
       </c>
@@ -1691,16 +1734,16 @@
         <v>63</v>
       </c>
       <c r="B9" s="16"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59" t="s">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
       <c r="K9" s="4" t="s">
         <v>27</v>
       </c>

</xml_diff>